<commit_message>
Correcciones de la estructura de la base de datos
</commit_message>
<xml_diff>
--- a/documentacion/DD Proyecto.xlsx
+++ b/documentacion/DD Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52664\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shavi\Downloads\visual\Proyecto\RBE\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C467BFB1-A06E-4110-A3DD-D5BCE986FB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46209B4-BF96-48FD-8E7E-59C9A9130545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="7776" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DICCIONARIO DE DATOS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="140">
   <si>
     <t>Número</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>Es el numero que identifica el tipo de pago</t>
+  </si>
+  <si>
+    <t>VIAJE_ASIENTO</t>
+  </si>
+  <si>
+    <t>Asociar el estado de un asiento en un viaje especifico.</t>
   </si>
 </sst>
 </file>
@@ -884,24 +890,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:F149"/>
+  <dimension ref="A4:F155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="2"/>
-    <col min="2" max="2" width="16.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" style="2"/>
-    <col min="5" max="5" width="11.08984375" style="3"/>
-    <col min="6" max="6" width="33.36328125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="11.08984375" style="2"/>
+    <col min="1" max="1" width="11.109375" style="2"/>
+    <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="2"/>
+    <col min="5" max="5" width="11.109375" style="3"/>
+    <col min="6" max="6" width="33.33203125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="11.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>75</v>
       </c>
@@ -909,7 +915,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>93</v>
       </c>
@@ -917,7 +923,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -937,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -955,7 +961,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -975,7 +981,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -993,7 +999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>5</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>6</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>75</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>93</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>1</v>
       </c>
@@ -1101,7 +1107,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>2</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>3</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>4</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>5</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>6</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>7</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>75</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>93</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>1</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>2</v>
       </c>
@@ -1291,7 +1297,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>75</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>93</v>
       </c>
@@ -1307,7 +1313,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>2</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>75</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>93</v>
       </c>
@@ -1383,7 +1389,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>0</v>
       </c>
@@ -1403,7 +1409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>1</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>2</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>3</v>
       </c>
@@ -1459,7 +1465,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>75</v>
       </c>
@@ -1467,7 +1473,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>93</v>
       </c>
@@ -1475,7 +1481,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>1</v>
       </c>
@@ -1513,7 +1519,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>2</v>
       </c>
@@ -1531,7 +1537,7 @@
       </c>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>3</v>
       </c>
@@ -1549,7 +1555,7 @@
       </c>
       <c r="F49" s="9"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>75</v>
       </c>
@@ -1557,7 +1563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>93</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>1</v>
       </c>
@@ -1601,7 +1607,7 @@
       </c>
       <c r="F54" s="9"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>2</v>
       </c>
@@ -1619,7 +1625,7 @@
       </c>
       <c r="F55" s="9"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>3</v>
       </c>
@@ -1637,7 +1643,7 @@
       </c>
       <c r="F56" s="9"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>75</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>93</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>0</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>1</v>
       </c>
@@ -1689,7 +1695,7 @@
       </c>
       <c r="F61" s="9"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>2</v>
       </c>
@@ -1707,7 +1713,7 @@
       </c>
       <c r="F62" s="9"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>3</v>
       </c>
@@ -1725,7 +1731,7 @@
       </c>
       <c r="F63" s="9"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>4</v>
       </c>
@@ -1743,7 +1749,7 @@
       </c>
       <c r="F64" s="9"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>5</v>
       </c>
@@ -1761,7 +1767,7 @@
       </c>
       <c r="F65" s="9"/>
     </row>
-    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>6</v>
       </c>
@@ -1779,7 +1785,7 @@
       </c>
       <c r="F66" s="9"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>75</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
         <v>93</v>
       </c>
@@ -1795,7 +1801,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>0</v>
       </c>
@@ -1815,7 +1821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>1</v>
       </c>
@@ -1833,7 +1839,7 @@
       </c>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="7">
         <v>2</v>
       </c>
@@ -1851,7 +1857,7 @@
       </c>
       <c r="F72" s="9"/>
     </row>
-    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>3</v>
       </c>
@@ -1867,7 +1873,7 @@
       </c>
       <c r="F73" s="9"/>
     </row>
-    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>4</v>
       </c>
@@ -1883,7 +1889,7 @@
       </c>
       <c r="F74" s="9"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>75</v>
       </c>
@@ -1891,7 +1897,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>93</v>
       </c>
@@ -1899,7 +1905,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>1</v>
       </c>
@@ -1935,7 +1941,7 @@
       </c>
       <c r="F79" s="9"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>2</v>
       </c>
@@ -1951,7 +1957,7 @@
       </c>
       <c r="F80" s="9"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>3</v>
       </c>
@@ -1967,7 +1973,7 @@
       </c>
       <c r="F81" s="9"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>4</v>
       </c>
@@ -1983,7 +1989,7 @@
       </c>
       <c r="F82" s="9"/>
     </row>
-    <row r="83" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>5</v>
       </c>
@@ -2001,7 +2007,7 @@
       </c>
       <c r="F83" s="9"/>
     </row>
-    <row r="84" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>6</v>
       </c>
@@ -2017,7 +2023,7 @@
       </c>
       <c r="F84" s="9"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
         <v>75</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>93</v>
       </c>
@@ -2033,7 +2039,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>1</v>
       </c>
@@ -2069,7 +2075,7 @@
       </c>
       <c r="F89" s="8"/>
     </row>
-    <row r="90" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="7">
         <v>2</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>3</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
         <v>75</v>
       </c>
@@ -2115,7 +2121,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
         <v>93</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>0</v>
       </c>
@@ -2143,7 +2149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>1</v>
       </c>
@@ -2159,7 +2165,7 @@
       </c>
       <c r="F96" s="9"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>2</v>
       </c>
@@ -2175,7 +2181,7 @@
       </c>
       <c r="F97" s="9"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
         <v>3</v>
       </c>
@@ -2191,7 +2197,7 @@
       </c>
       <c r="F98" s="9"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
         <v>75</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
         <v>93</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="7">
         <v>1</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="7">
         <v>2</v>
       </c>
@@ -2263,7 +2269,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="7">
         <v>3</v>
       </c>
@@ -2281,7 +2287,7 @@
       </c>
       <c r="F105" s="9"/>
     </row>
-    <row r="106" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="7">
         <v>4</v>
       </c>
@@ -2297,7 +2303,7 @@
       </c>
       <c r="F106" s="9"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
         <v>75</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
         <v>93</v>
       </c>
@@ -2313,7 +2319,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>0</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="7">
         <v>1</v>
       </c>
@@ -2349,7 +2355,7 @@
       </c>
       <c r="F111" s="9"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="7">
         <v>2</v>
       </c>
@@ -2367,7 +2373,7 @@
       </c>
       <c r="F112" s="9"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="7">
         <v>3</v>
       </c>
@@ -2385,7 +2391,7 @@
       </c>
       <c r="F113" s="9"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="7">
         <v>4</v>
       </c>
@@ -2401,7 +2407,7 @@
       <c r="E114" s="8"/>
       <c r="F114" s="9"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="7">
         <v>5</v>
       </c>
@@ -2417,7 +2423,7 @@
       </c>
       <c r="F115" s="9"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="7">
         <v>6</v>
       </c>
@@ -2431,7 +2437,7 @@
       <c r="E116" s="8"/>
       <c r="F116" s="9"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
         <v>75</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
         <v>93</v>
       </c>
@@ -2447,7 +2453,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>0</v>
       </c>
@@ -2467,7 +2473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="7">
         <v>1</v>
       </c>
@@ -2485,7 +2491,7 @@
       </c>
       <c r="F121" s="9"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="7">
         <v>2</v>
       </c>
@@ -2501,7 +2507,7 @@
       </c>
       <c r="F122" s="9"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="7">
         <v>3</v>
       </c>
@@ -2517,7 +2523,7 @@
       </c>
       <c r="F123" s="9"/>
     </row>
-    <row r="124" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="7">
         <v>4</v>
       </c>
@@ -2533,7 +2539,7 @@
       </c>
       <c r="F124" s="9"/>
     </row>
-    <row r="125" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="7">
         <v>5</v>
       </c>
@@ -2549,7 +2555,7 @@
       </c>
       <c r="F125" s="9"/>
     </row>
-    <row r="126" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="7">
         <v>6</v>
       </c>
@@ -2565,7 +2571,7 @@
       </c>
       <c r="F126" s="9"/>
     </row>
-    <row r="127" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="7">
         <v>7</v>
       </c>
@@ -2581,7 +2587,7 @@
       </c>
       <c r="F127" s="9"/>
     </row>
-    <row r="128" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="7">
         <v>8</v>
       </c>
@@ -2599,7 +2605,7 @@
       </c>
       <c r="F128" s="9"/>
     </row>
-    <row r="129" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="7">
         <v>9</v>
       </c>
@@ -2615,7 +2621,7 @@
       </c>
       <c r="F129" s="9"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="12" t="s">
         <v>75</v>
       </c>
@@ -2623,7 +2629,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="12" t="s">
         <v>93</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>0</v>
       </c>
@@ -2651,7 +2657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="7">
         <v>1</v>
       </c>
@@ -2669,7 +2675,7 @@
       </c>
       <c r="F134" s="9"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="7">
         <v>2</v>
       </c>
@@ -2685,7 +2691,7 @@
       </c>
       <c r="F135" s="9"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="7">
         <v>3</v>
       </c>
@@ -2701,7 +2707,7 @@
       </c>
       <c r="F136" s="9"/>
     </row>
-    <row r="137" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="7">
         <v>4</v>
       </c>
@@ -2717,7 +2723,7 @@
       </c>
       <c r="F137" s="9"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="12" t="s">
         <v>75</v>
       </c>
@@ -2725,7 +2731,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="12" t="s">
         <v>93</v>
       </c>
@@ -2733,7 +2739,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>0</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="7">
         <v>1</v>
       </c>
@@ -2769,7 +2775,7 @@
       </c>
       <c r="F142" s="9"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="7">
         <v>2</v>
       </c>
@@ -2787,7 +2793,7 @@
       </c>
       <c r="F143" s="9"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="7">
         <v>3</v>
       </c>
@@ -2805,7 +2811,7 @@
       </c>
       <c r="F144" s="9"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="7">
         <v>4</v>
       </c>
@@ -2821,7 +2827,7 @@
       <c r="E145" s="8"/>
       <c r="F145" s="9"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="7">
         <v>5</v>
       </c>
@@ -2837,7 +2843,7 @@
       </c>
       <c r="F146" s="9"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="7">
         <v>6</v>
       </c>
@@ -2855,7 +2861,7 @@
       </c>
       <c r="F147" s="9"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="7">
         <v>7</v>
       </c>
@@ -2873,7 +2879,7 @@
       </c>
       <c r="F148" s="9"/>
     </row>
-    <row r="149" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="7">
         <v>8</v>
       </c>
@@ -2888,6 +2894,74 @@
         <v>72</v>
       </c>
       <c r="F149" s="9"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="7">
+        <v>1</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D154" s="7"/>
+      <c r="E154" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F154" s="9"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="7">
+        <v>2</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D155" s="7"/>
+      <c r="E155" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F155" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>